<commit_message>
agregado cumpleaños doctor estrada
</commit_message>
<xml_diff>
--- a/cumpleaniosOtros.xlsx
+++ b/cumpleaniosOtros.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>DIA</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>LAURA QUINTERO SALINAS</t>
+  </si>
+  <si>
+    <t>HERNANDO ESTRADA PACHECO</t>
   </si>
 </sst>
 </file>
@@ -386,7 +389,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,6 +493,17 @@
         <v>10</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>11</v>
+      </c>
+    </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" s="1"/>
     </row>

</xml_diff>